<commit_message>
Update with new AIC, MSE, deviance
</commit_message>
<xml_diff>
--- a/results/hindcast_models.xlsx
+++ b/results/hindcast_models.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\Bering_LarvalForecast\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDE7897-995F-4B64-9BB4-19442B5F8F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6B4ABE-93AD-46EA-B0E0-BD33F4A5DFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MSE Comparison" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
   <si>
     <t>Here we are looking to see if the base model has higher error. That model doesn't include a varying coefficient term</t>
   </si>
@@ -786,29 +786,89 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
+      <t>) + te(lat, lon, by = T) + ɛ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>lat,lon</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ln(count) = re(y) + s(lat, lon) + s(J</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>lat,lon</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>) + s(SST</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>lat,lon</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
       <t>) + s(SSS</t>
     </r>
     <r>
       <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>lat,lon</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>) + te(lat, lon, by = T) + ɛ</t>
-    </r>
-    <r>
-      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>lat,lon</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>) + s(J, by = T) + ɛ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <vertAlign val="subscript"/>
         <sz val="11"/>
         <color theme="1"/>
@@ -871,7 +931,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -896,6 +956,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -909,7 +975,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -934,7 +1000,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -961,6 +1026,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1297,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1324,54 +1416,54 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="C4" s="20">
-        <v>0.12</v>
+      <c r="B4" s="19">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C4" s="19">
+        <v>0.11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="20">
-        <v>0.2</v>
-      </c>
-      <c r="C5" s="20">
-        <v>0.21</v>
+      <c r="B5" s="19">
+        <v>0.24</v>
+      </c>
+      <c r="C5" s="19">
+        <v>0.26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="19">
         <v>0.09</v>
       </c>
-      <c r="C6" s="20">
-        <v>0.11</v>
+      <c r="C6" s="19">
+        <v>0.12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="20">
-        <v>0.35</v>
-      </c>
-      <c r="C7" s="20">
-        <v>0.41</v>
+      <c r="B7" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="C7" s="19">
+        <v>0.37</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="19">
         <v>0.11</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="19">
         <v>0.18</v>
       </c>
     </row>
@@ -1379,10 +1471,10 @@
       <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="C9" s="20">
+      <c r="B9" s="19">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C9" s="19">
         <v>0.35</v>
       </c>
     </row>
@@ -1390,50 +1482,62 @@
       <c r="A10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
+      <c r="B10" s="19">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C10" s="19">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
+      <c r="B11" s="19">
+        <v>0.11</v>
+      </c>
+      <c r="C11" s="19">
+        <v>0.13</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
+      <c r="B12" s="19">
+        <v>0.12</v>
+      </c>
+      <c r="C12" s="19">
+        <v>0.12</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1444,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85362540-AC5F-4C2A-96D6-CE4627EBF886}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D34" sqref="B34:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1456,16 +1560,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1476,40 +1580,60 @@
       <c r="B2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
+      <c r="C2" s="5">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="D2" s="6">
+        <v>33301</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A3" s="7"/>
       <c r="B3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
+      <c r="C3" s="5">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="D3" s="6">
+        <v>33128</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.45">
+      <c r="C4" s="5">
+        <v>0.502</v>
+      </c>
+      <c r="D4" s="6">
+        <v>33009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.4">
       <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="D5" s="6">
+        <v>32825</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.45">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.4">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
+      <c r="C6" s="24">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="D6" s="25">
+        <v>32829</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
@@ -1518,32 +1642,48 @@
       <c r="B7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
+      <c r="C7" s="11">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="D7" s="12">
+        <v>30602</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A8" s="13"/>
       <c r="B8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
+      <c r="C8" s="11">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="D8" s="12">
+        <v>29857</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A9" s="9"/>
       <c r="B9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="12"/>
+      <c r="C9" s="18">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="D9" s="12">
+        <v>29569</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.4">
       <c r="A10" s="9"/>
       <c r="B10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
+      <c r="C10" s="22">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="D10" s="23">
+        <v>29457</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
@@ -1552,32 +1692,48 @@
       <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
+      <c r="C11" s="5">
+        <v>0.436</v>
+      </c>
+      <c r="D11" s="6">
+        <v>14919</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A12" s="7"/>
       <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
+      <c r="C12" s="5">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="D12" s="6">
+        <v>14765</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
+      <c r="C13" s="5">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="D13" s="6">
+        <v>14709</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.4">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
+      <c r="C14" s="20">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="D14" s="21">
+        <v>14603</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
@@ -1586,32 +1742,48 @@
       <c r="B15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12"/>
+      <c r="C15" s="11">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="D15" s="12">
+        <v>11038</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A16" s="13"/>
       <c r="B16" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12"/>
+      <c r="C16" s="11">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="D16" s="12">
+        <v>10223</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A17" s="9"/>
       <c r="B17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12"/>
+      <c r="C17" s="11">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="D17" s="12">
+        <v>9978</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.4">
       <c r="A18" s="9"/>
       <c r="B18" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="24"/>
+      <c r="C18" s="22">
+        <v>0.69</v>
+      </c>
+      <c r="D18" s="23">
+        <v>9778</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
@@ -1620,32 +1792,48 @@
       <c r="B19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
+      <c r="C19" s="5">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="D19" s="6">
+        <v>10360</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A20" s="7"/>
       <c r="B20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
+      <c r="C20" s="5">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="D20" s="6">
+        <v>10291</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
+      <c r="C21" s="5">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="D21" s="6">
+        <v>10141</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.4">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="22"/>
+      <c r="C22" s="20">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="D22" s="21">
+        <v>10002</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
@@ -1654,32 +1842,48 @@
       <c r="B23" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12"/>
+      <c r="C23" s="11">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="D23" s="12">
+        <v>15412</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A24" s="13"/>
       <c r="B24" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="12"/>
+      <c r="C24" s="11">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="D24" s="12">
+        <v>14441</v>
+      </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A25" s="9"/>
       <c r="B25" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="12"/>
+      <c r="C25" s="11">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="D25" s="12">
+        <v>14353</v>
+      </c>
     </row>
     <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.4">
       <c r="A26" s="9"/>
       <c r="B26" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="24"/>
+      <c r="C26" s="22">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="D26" s="23">
+        <v>14092</v>
+      </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
@@ -1688,32 +1892,48 @@
       <c r="B27" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="6"/>
+      <c r="C27" s="5">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="D27" s="6">
+        <v>7441</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A28" s="7"/>
       <c r="B28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="6"/>
+      <c r="C28" s="5">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="D28" s="6">
+        <v>7064</v>
+      </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A29" s="3"/>
       <c r="B29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.45">
+      <c r="C29" s="5">
+        <v>0.753</v>
+      </c>
+      <c r="D29" s="6">
+        <v>6721</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.4">
       <c r="A30" s="3"/>
-      <c r="B30" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
+      <c r="B30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="20">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="D30" s="21">
+        <v>6655</v>
+      </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
@@ -1722,66 +1942,98 @@
       <c r="B31" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="12"/>
+      <c r="C31" s="11">
+        <v>0.439</v>
+      </c>
+      <c r="D31" s="12">
+        <v>15812</v>
+      </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A32" s="13"/>
       <c r="B32" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="12"/>
+      <c r="C32" s="11">
+        <v>0.49</v>
+      </c>
+      <c r="D32" s="12">
+        <v>15558</v>
+      </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.45">
       <c r="A33" s="9"/>
       <c r="B33" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="12"/>
-    </row>
-    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.45">
+      <c r="C33" s="11">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="D33" s="12">
+        <v>15443</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.4">
       <c r="A34" s="9"/>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="22">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="D34" s="23">
+        <v>15397</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.45">
+      <c r="A35" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="28">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D35" s="29">
+        <v>9004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.45">
+      <c r="A36" s="30"/>
+      <c r="B36" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="28">
+        <v>51.5</v>
+      </c>
+      <c r="D36" s="29">
+        <v>8883</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.4">
+      <c r="A37" s="27"/>
+      <c r="B37" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="33">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="D37" s="34">
+        <v>8685</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.45">
+      <c r="A38" s="27"/>
+      <c r="B38" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="12"/>
-    </row>
-    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.45">
-      <c r="A35" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="12"/>
-    </row>
-    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.45">
-      <c r="A36" s="13"/>
-      <c r="B36" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="12"/>
-    </row>
-    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.45">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="12"/>
-    </row>
-    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.45">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="13"/>
+      <c r="C38" s="32">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="D38" s="31">
+        <v>8704</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>

</xml_diff>

<commit_message>
Update figures and tables
</commit_message>
<xml_diff>
--- a/results/hindcast_models.xlsx
+++ b/results/hindcast_models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\Bering_LarvalForecast\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6B4ABE-93AD-46EA-B0E0-BD33F4A5DFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE88568-6F68-47C4-B2F1-21E7F226B3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MSE Comparison" sheetId="1" r:id="rId1"/>
@@ -1389,7 +1389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -1548,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85362540-AC5F-4C2A-96D6-CE4627EBF886}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D34" sqref="B34:D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1616,10 +1616,10 @@
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="20">
         <v>0.53100000000000003</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="21">
         <v>32825</v>
       </c>
     </row>

</xml_diff>